<commit_message>
week 16 injury + weather data updates
</commit_message>
<xml_diff>
--- a/data/external/Weather.xlsx
+++ b/data/external/Weather.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johno\Documents\Sports Research\NFL\data\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johno\Documents\nfl-dashboard\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5287486-65DD-4FB0-87B9-B7371EE9D129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18236DF-A53D-4682-A306-9DF66AE93156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="6636" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 13" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81989515-5A8F-4B87-BDB8-A67067333F81}" name="Table2" displayName="Table2" ref="A1:C17" totalsRowShown="0">
   <autoFilter ref="A1:C17" xr:uid="{81989515-5A8F-4B87-BDB8-A67067333F81}">
     <filterColumn colId="2">
-      <filters blank="1"/>
+      <filters>
+        <filter val="Good"/>
+        <filter val="Mildly Cold"/>
+        <filter val="Rainy, Slight Wind"/>
+        <filter val="Slight Snow, Mildly Cold"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="3">
@@ -524,12 +529,12 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -548,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -556,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -564,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -572,7 +577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -580,7 +585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -588,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -596,7 +601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -604,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -612,7 +617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -620,7 +625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -628,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -636,7 +641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -644,7 +649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -652,7 +657,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -660,7 +665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -681,12 +686,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -708,7 +713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -719,7 +724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -730,7 +735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -741,7 +746,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -752,7 +757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -763,7 +768,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -774,7 +779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -785,7 +790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -796,7 +801,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -807,7 +812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -818,7 +823,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -829,7 +834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -853,12 +858,12 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -880,7 +885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -891,7 +896,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -902,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -913,7 +918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -924,7 +929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -935,7 +940,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -946,7 +951,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -957,7 +962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -968,7 +973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -979,7 +984,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -990,7 +995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1001,7 +1006,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1012,7 +1017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1028,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1061,12 +1066,12 @@
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1088,7 +1093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1110,7 +1115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1126,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1137,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1148,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1154,7 +1159,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1192,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1214,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1269,9 +1274,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1298,7 +1303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1306,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1330,7 +1335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1362,7 +1367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1370,7 +1375,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1394,7 +1399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1423,9 +1428,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1444,7 +1449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1452,7 +1457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1484,7 +1489,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1492,7 +1497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1500,7 +1505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1508,7 +1513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1524,7 +1529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1532,7 +1537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1540,7 +1545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1548,7 +1553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1556,7 +1561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>

</xml_diff>